<commit_message>
added Sokhna new design
</commit_message>
<xml_diff>
--- a/WatanyaPingTester/bin/Debug/data/sokhna_scheme.xlsx
+++ b/WatanyaPingTester/bin/Debug/data/sokhna_scheme.xlsx
@@ -310,13 +310,13 @@
     <t>192.168.1.169</t>
   </si>
   <si>
-    <t>192.168.186</t>
-  </si>
-  <si>
     <t>192.168.1.187</t>
   </si>
   <si>
     <t>Previous IP</t>
+  </si>
+  <si>
+    <t>192.168.1.186</t>
   </si>
 </sst>
 </file>
@@ -675,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -710,7 +710,7 @@
         <v>57</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2147,7 +2147,7 @@
         <v>71</v>
       </c>
       <c r="C64" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>66</v>
@@ -2193,7 +2193,7 @@
         <v>71</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>66</v>

</xml_diff>